<commit_message>
Updated CLR to prep for test ingest
</commit_message>
<xml_diff>
--- a/whale-wave/OLR/standard_input_whale_wave.xlsx
+++ b/whale-wave/OLR/standard_input_whale_wave.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23790" windowHeight="11835" tabRatio="351"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23790" windowHeight="7275" tabRatio="351"/>
   </bookViews>
   <sheets>
     <sheet name="Item description" sheetId="9" r:id="rId1"/>
@@ -133,7 +133,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="686" uniqueCount="655">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="688" uniqueCount="657">
   <si>
     <t>text</t>
   </si>
@@ -2098,6 +2098,12 @@
   </si>
   <si>
     <t>Keen, EM, Wray, J, Meuter, H, Thompson, K-L, and Picard, CR. (Accepted 2016) "Whale Wave": Shifting strategies structure complex use of critical fjord habitat by fin whales. Marine Ecology Progress Series.</t>
+  </si>
+  <si>
+    <t>This archive file contains all the data for this collection. After extraction, in each folder you will find PDF documents that detail the data processing and analysis used in their respective topics. These PDFs guide the user through the location and content of the data and R scripts within the subfolders.</t>
+  </si>
+  <si>
+    <t>List of necessary R packages/versions</t>
   </si>
 </sst>
 </file>
@@ -3166,10 +3172,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y4"/>
+  <dimension ref="A1:Z4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3184,11 +3190,11 @@
     <col min="16" max="17" width="45.5703125" style="3" customWidth="1"/>
     <col min="18" max="18" width="14.85546875" style="3" customWidth="1"/>
     <col min="19" max="19" width="15.140625" style="3" customWidth="1"/>
-    <col min="20" max="23" width="39.140625" style="3" customWidth="1"/>
-    <col min="24" max="25" width="42.85546875" style="3" customWidth="1"/>
+    <col min="20" max="24" width="39.140625" style="3" customWidth="1"/>
+    <col min="25" max="26" width="42.85546875" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
         <v>338</v>
       </c>
@@ -3256,22 +3262,28 @@
         <v>627</v>
       </c>
       <c r="W1" s="16" t="s">
+        <v>507</v>
+      </c>
+      <c r="X1" s="16" t="s">
         <v>628</v>
       </c>
-      <c r="X1" s="16" t="s">
+      <c r="Y1" s="16" t="s">
         <v>460</v>
       </c>
-      <c r="Y1" s="16" t="s">
+      <c r="Z1" s="16" t="s">
         <v>455</v>
       </c>
     </row>
-    <row r="2" spans="1:25" ht="180" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:26" ht="180" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>631</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>485</v>
       </c>
+      <c r="E2" s="3" t="s">
+        <v>634</v>
+      </c>
       <c r="G2" s="3" t="s">
         <v>651</v>
       </c>
@@ -3317,17 +3329,17 @@
       <c r="V2" s="3" t="s">
         <v>653</v>
       </c>
-      <c r="W2" s="3" t="s">
+      <c r="X2" s="3" t="s">
         <v>654</v>
       </c>
-      <c r="X2" s="3" t="s">
+      <c r="Y2" s="3" t="s">
         <v>642</v>
       </c>
-      <c r="Y2" s="3" t="s">
+      <c r="Z2" s="3" t="s">
         <v>652</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" ht="120" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>631</v>
       </c>
@@ -3340,17 +3352,20 @@
       <c r="D3" s="3" t="s">
         <v>403</v>
       </c>
-      <c r="E3" s="3" t="s">
-        <v>634</v>
-      </c>
       <c r="F3" s="3" t="s">
         <v>358</v>
       </c>
       <c r="G3" s="3" t="s">
         <v>635</v>
       </c>
-    </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="U3" s="3" t="s">
+        <v>655</v>
+      </c>
+      <c r="W3" s="3" t="s">
+        <v>656</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>631</v>
       </c>
@@ -3362,9 +3377,6 @@
       </c>
       <c r="D4" s="3" t="s">
         <v>384</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>0</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>358</v>
@@ -3411,7 +3423,7 @@
           <x14:formula1>
             <xm:f>'Select-a-header values'!$G$1:$G$17</xm:f>
           </x14:formula1>
-          <xm:sqref>X1:Y1</xm:sqref>
+          <xm:sqref>Y1:Z1</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid header" error="Please select a header from the drop-down list" prompt="Please select a header from the drop-down list">
           <x14:formula1>
@@ -3423,7 +3435,7 @@
           <x14:formula1>
             <xm:f>'Select-a-header values'!$E$1:$E$34</xm:f>
           </x14:formula1>
-          <xm:sqref>T1:W1</xm:sqref>
+          <xm:sqref>T1:X1</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
Updated OLR to prep for test ingest
</commit_message>
<xml_diff>
--- a/whale-wave/OLR/standard_input_whale_wave.xlsx
+++ b/whale-wave/OLR/standard_input_whale_wave.xlsx
@@ -133,7 +133,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="688" uniqueCount="657">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="689" uniqueCount="658">
   <si>
     <t>text</t>
   </si>
@@ -2100,10 +2100,13 @@
     <t>Keen, EM, Wray, J, Meuter, H, Thompson, K-L, and Picard, CR. (Accepted 2016) "Whale Wave": Shifting strategies structure complex use of critical fjord habitat by fin whales. Marine Ecology Progress Series.</t>
   </si>
   <si>
-    <t>This archive file contains all the data for this collection. After extraction, in each folder you will find PDF documents that detail the data processing and analysis used in their respective topics. These PDFs guide the user through the location and content of the data and R scripts within the subfolders.</t>
-  </si>
-  <si>
     <t>List of necessary R packages/versions</t>
+  </si>
+  <si>
+    <t>This archive file contains all the data in the collection.</t>
+  </si>
+  <si>
+    <t>After extraction, in each folder you will find PDF documents that detail the data processing and analysis used in their respective topics. These PDFs guide the user through the location and content of the data and R scripts within the subfolders.</t>
   </si>
 </sst>
 </file>
@@ -2826,42 +2829,7 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="5">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC0D494"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC3D69A"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFACD575"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
@@ -3174,8 +3142,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
+      <selection activeCell="T3" sqref="T3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3339,7 +3307,7 @@
         <v>652</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="120" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" ht="105" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>631</v>
       </c>
@@ -3358,11 +3326,14 @@
       <c r="G3" s="3" t="s">
         <v>635</v>
       </c>
+      <c r="T3" s="3" t="s">
+        <v>656</v>
+      </c>
       <c r="U3" s="3" t="s">
+        <v>657</v>
+      </c>
+      <c r="W3" s="3" t="s">
         <v>655</v>
-      </c>
-      <c r="W3" s="3" t="s">
-        <v>656</v>
       </c>
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added technical details to the data
</commit_message>
<xml_diff>
--- a/whale-wave/OLR/standard_input_whale_wave.xlsx
+++ b/whale-wave/OLR/standard_input_whale_wave.xlsx
@@ -2100,13 +2100,18 @@
     <t>Keen, EM, Wray, J, Meuter, H, Thompson, K-L, and Picard, CR. (Accepted 2016) "Whale Wave": Shifting strategies structure complex use of critical fjord habitat by fin whales. Marine Ecology Progress Series.</t>
   </si>
   <si>
-    <t>List of necessary R packages/versions</t>
-  </si>
-  <si>
     <t>This archive file contains all the data in the collection.</t>
   </si>
   <si>
     <t>After extraction, in each folder you will find PDF documents that detail the data processing and analysis used in their respective topics. These PDFs guide the user through the location and content of the data and R scripts within the subfolders.</t>
+  </si>
+  <si>
+    <t>This data was produced with R version 3.1.2, and the following R packages and versions:
+PBSMapping v 2.67.60
+The 'bangarang' package - &lt;a href="https://github.com/ericmkeen/bangarang"&gt;GitHub link&lt;/a&gt;
+swfscMisc, v. 1.0.3
+MASS v.7.3-35
+mgcv, v1.8-3</t>
   </si>
 </sst>
 </file>
@@ -3142,8 +3147,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
-      <selection activeCell="T3" sqref="T3"/>
+    <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
+      <selection activeCell="W3" sqref="W3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3307,7 +3312,7 @@
         <v>652</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="105" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" ht="150" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>631</v>
       </c>
@@ -3327,13 +3332,13 @@
         <v>635</v>
       </c>
       <c r="T3" s="3" t="s">
+        <v>655</v>
+      </c>
+      <c r="U3" s="3" t="s">
         <v>656</v>
       </c>
-      <c r="U3" s="3" t="s">
+      <c r="W3" s="3" t="s">
         <v>657</v>
-      </c>
-      <c r="W3" s="3" t="s">
-        <v>655</v>
       </c>
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Moved a subject to scientific name
</commit_message>
<xml_diff>
--- a/whale-wave/OLR/standard_input_whale_wave.xlsx
+++ b/whale-wave/OLR/standard_input_whale_wave.xlsx
@@ -133,7 +133,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="677" uniqueCount="652">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="679" uniqueCount="653">
   <si>
     <t>text</t>
   </si>
@@ -2090,10 +2090,13 @@
 mgcv, v1.8-3</t>
   </si>
   <si>
-    <t>Humpback whale | Megaptera novaeangliae | Habitat use | Habitat model | Gitga'at First Nation</t>
-  </si>
-  <si>
     <t>Keen, Eric M; Wray, Janie; Meuter, Hermann; Thompson, Kim-Ly; Barlow, Jay P; Picard, Chris R (2017): Data from: "Whale Wave": shifting strategies structure the complex use of critical fjord habitats by humpbacks. UC San Diego Library Digital Collections.</t>
+  </si>
+  <si>
+    <t>Humpback whale | Habitat use | Habitat model | Gitga'at First Nation</t>
+  </si>
+  <si>
+    <t>Megaptera novaeangliae</t>
   </si>
 </sst>
 </file>
@@ -3127,10 +3130,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T4"/>
+  <dimension ref="A1:U4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="N2" sqref="N2"/>
+    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
+      <selection activeCell="S2" sqref="S2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3146,10 +3149,10 @@
     <col min="11" max="11" width="14.85546875" style="3" customWidth="1"/>
     <col min="12" max="12" width="15.140625" style="3" customWidth="1"/>
     <col min="13" max="18" width="39.140625" style="3" customWidth="1"/>
-    <col min="19" max="20" width="42.85546875" style="3" customWidth="1"/>
+    <col min="19" max="21" width="42.85546875" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
         <v>338</v>
       </c>
@@ -3208,10 +3211,13 @@
         <v>460</v>
       </c>
       <c r="T1" s="16" t="s">
+        <v>510</v>
+      </c>
+      <c r="U1" s="16" t="s">
         <v>455</v>
       </c>
     </row>
-    <row r="2" spans="1:20" ht="180" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" ht="180" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>631</v>
       </c>
@@ -3243,7 +3249,7 @@
         <v>641</v>
       </c>
       <c r="N2" s="3" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="P2" s="3" t="s">
         <v>645</v>
@@ -3252,13 +3258,16 @@
         <v>646</v>
       </c>
       <c r="S2" s="3" t="s">
-        <v>650</v>
+        <v>651</v>
       </c>
       <c r="T2" s="3" t="s">
+        <v>652</v>
+      </c>
+      <c r="U2" s="3" t="s">
         <v>644</v>
       </c>
     </row>
-    <row r="3" spans="1:20" ht="150" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" ht="150" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>631</v>
       </c>
@@ -3287,7 +3296,7 @@
         <v>649</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>631</v>
       </c>
@@ -3345,7 +3354,7 @@
           <x14:formula1>
             <xm:f>'Select-a-header values'!$G$1:$G$17</xm:f>
           </x14:formula1>
-          <xm:sqref>S1:T1</xm:sqref>
+          <xm:sqref>S1:U1</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid header" error="Please select a header from the drop-down list" prompt="Please select a header from the drop-down list">
           <x14:formula1>

</xml_diff>